<commit_message>
some changes to design + lab.js
</commit_message>
<xml_diff>
--- a/design/design.xlsx
+++ b/design/design.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\SPR_online\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\SPR_online\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E10735-F76F-429D-970B-87A6A88480EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541BD8CB-356F-4599-BFC6-B0D37252E938}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$E$73</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="9">
-  <si>
-    <t>Item</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="14">
   <si>
     <t>cond</t>
   </si>
@@ -52,6 +52,24 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -113,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -127,6 +145,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,94 +429,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="2"/>
+    <col min="1" max="5" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D4" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -507,106 +551,133 @@
       <c r="D7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C11" s="3"/>
       <c r="D11" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>2</v>
       </c>
@@ -619,202 +690,257 @@
       <c r="D15" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>3</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C16" s="4"/>
       <c r="D16" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>8</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C19" s="4"/>
       <c r="D19" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>7</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D20" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>8</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>9</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>10</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D23" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>11</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D24" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>12</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>1</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D26" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>3</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="D28" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>4</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D29" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>5</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C30" s="3"/>
       <c r="D30" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>6</v>
       </c>
@@ -822,18 +948,21 @@
         <v>4</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D31" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>7</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>7</v>
@@ -841,36 +970,43 @@
       <c r="D32" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>8</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C33" s="3"/>
       <c r="D33" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>9</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D34" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>10</v>
       </c>
@@ -878,103 +1014,129 @@
         <v>5</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>11</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C36" s="3"/>
       <c r="D36" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>12</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D37" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>1</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>2</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="4"/>
+      <c r="C39" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D39" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>3</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D40" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>4</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>5</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>6</v>
       </c>
@@ -982,74 +1144,85 @@
         <v>5</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D43" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>7</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>8</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C44" s="4"/>
       <c r="D44" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>8</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D45" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>9</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D46" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>10</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C47" s="4"/>
       <c r="D47" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>11</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>7</v>
@@ -1057,36 +1230,45 @@
       <c r="D48" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>12</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D49" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>1</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D50" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>2</v>
       </c>
@@ -1094,74 +1276,85 @@
         <v>5</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D51" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>3</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C52" s="3"/>
       <c r="D52" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>4</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D53" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>5</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D54" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>6</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C55" s="3"/>
       <c r="D55" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>7</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>7</v>
@@ -1169,132 +1362,173 @@
       <c r="D56" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>8</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D57" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>9</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>10</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C59" s="3"/>
+      <c r="C59" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D59" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>11</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="D60" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>12</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>1</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D62" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>2</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>3</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D64" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>4</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D65" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>5</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>8</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C66" s="4"/>
       <c r="D66" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>6</v>
       </c>
@@ -1302,46 +1536,53 @@
         <v>4</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D67" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>7</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D68" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>8</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>8</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C69" s="4"/>
       <c r="D69" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>9</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>7</v>
@@ -1349,8 +1590,11 @@
       <c r="D70" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>10</v>
       </c>
@@ -1358,32 +1602,36 @@
         <v>5</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D71" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>11</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C72" s="4"/>
       <c r="D72" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>12</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>7</v>
@@ -1391,8 +1639,12 @@
       <c r="D73" s="4">
         <v>6</v>
       </c>
+      <c r="E73" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E73" xr:uid="{85C67D95-22D5-43F4-A8FB-7ACA18B11AF6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>